<commit_message>
added a few things
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daria\Desktop\ECG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Desktop\ECG\EKG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E215965-02A1-49C3-ADB5-17D0D9765707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5706E610-490B-4528-94FF-FDF81FD743E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E91AA3BF-2B3A-4C31-B2DD-C366AC706276}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E91AA3BF-2B3A-4C31-B2DD-C366AC706276}"/>
   </bookViews>
   <sheets>
     <sheet name="to buy" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="127">
   <si>
     <t>FC681374V</t>
   </si>
@@ -135,6 +135,314 @@
   </si>
   <si>
     <t>Potentiometer 20k</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>LibRef</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Supplier Part Number</t>
+  </si>
+  <si>
+    <t>0.1uF 0805</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, 15% TC, 0.1uF, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5</t>
+  </si>
+  <si>
+    <t>C0805 - XL</t>
+  </si>
+  <si>
+    <t>0.1uF 0805B104K500CT</t>
+  </si>
+  <si>
+    <t>Walsin Technologies</t>
+  </si>
+  <si>
+    <t>0805B104K500CT</t>
+  </si>
+  <si>
+    <t>1=0.0564, 10=0.0292, 100=0.0134, 1000=0.00388, 4000=0.00315, 8000=0.00305, 20000=0.00299, 40000=0.00295, 80000=0.00291, 160000=0.00289 (EUR)</t>
+  </si>
+  <si>
+    <t>TME</t>
+  </si>
+  <si>
+    <t>3.3uF 0805</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 10V, 10% +Tol, 10% -Tol, X5R, 15% TC, 3.3uF, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>3.3uF 0805X335K100CT</t>
+  </si>
+  <si>
+    <t>0805X335K100CT</t>
+  </si>
+  <si>
+    <t>1=0.1894, 5=0.1297, 10=0.1085, 50=0.0684, 100=0.0569, 250=0.0462, 500=0.0407, 3000=0.0325, 45000=0.0281, 99000=0.0276 (EUR)</t>
+  </si>
+  <si>
+    <t>1uF 0805</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 25V, 10% +Tol, 10% -Tol, X7R, 15% TC, 1uF, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>1uF 0805B105K250CT</t>
+  </si>
+  <si>
+    <t>0805B105K250CT</t>
+  </si>
+  <si>
+    <t>1=0.1133, 10=0.027, 1000=0.0203, 3000=0.0185, 6000=0.0169, 9000=0.0154, 60000=0.0133, 75000=0.0126, 90000=0.012, 99000=0.0116 (EUR)</t>
+  </si>
+  <si>
+    <t>22nF 0805</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor, Multilayer, Ceramic, 50V, 10% +Tol, 10% -Tol, X7R, 15% TC, 0.022uF, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>22nF 0805B223K500CT</t>
+  </si>
+  <si>
+    <t>0805B223K500CT</t>
+  </si>
+  <si>
+    <t>1=0.0855, 10=0.0209, 50=0.0147, 100=0.0129, 500=0.0097, 1000=0.0087, 3000=0.0075, 4000=0.0073, 8000=0.0067, 20000=0.0061 (EUR)</t>
+  </si>
+  <si>
+    <t>LM324N</t>
+  </si>
+  <si>
+    <t>Operational Amplifier, 4 Func, 9000uV Offset-Max, BIPolar, PDIP14</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>DIP14 -  socket</t>
+  </si>
+  <si>
+    <t>LM324N-Socketed</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>1=0.475, 10=0.333, 25=0.266, 100=0.238, 250=0.2, 500=0.18, 1000=0.166, 2500=0.154 (EUR)</t>
+  </si>
+  <si>
+    <t>LM324N-TI</t>
+  </si>
+  <si>
+    <t>LM7805CT</t>
+  </si>
+  <si>
+    <t>Fixed Positive Standard Regulator, 5VBIPolar, PSFM3</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>TO-220-3</t>
+  </si>
+  <si>
+    <t>LM7805CT/NOPB</t>
+  </si>
+  <si>
+    <t>1=1.21, 45=1.13, 90=1.07, 270=0.92, 450=0.84, 540=0.81, 675=0.78, 1035=0.77 (EUR)</t>
+  </si>
+  <si>
+    <t>961102-6404-AR-HDR2-SIL</t>
+  </si>
+  <si>
+    <t>Pin Strip Header 2PIN SIL</t>
+  </si>
+  <si>
+    <t>J2, J3, J7</t>
+  </si>
+  <si>
+    <t>HDR1X2-961102-6404-AR</t>
+  </si>
+  <si>
+    <t>HDR2x1-961102-6404-AR</t>
+  </si>
+  <si>
+    <t>DC Power Plug or Jack.                     Contact Resistance: 30m max. W_x000D_
+Insulation Resistance: 100M min. at DC 500V W_x000D_
+Dielectric Withstand Voltage: AC 500V for 1 minute</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>Cliff</t>
+  </si>
+  <si>
+    <t>1=1.25, 20=1.09, 100=0.97, 500=0.76 (EUR)</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>5mm Green LED</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED 5mm THT</t>
+  </si>
+  <si>
+    <t>LED G</t>
+  </si>
+  <si>
+    <t>30k 0805</t>
+  </si>
+  <si>
+    <t>Fixed Resistor, Metal Glaze/thick Film, 0.125W, 30000ohm, 150V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>R1, R2, R4, R5</t>
+  </si>
+  <si>
+    <t>R0805 - XL</t>
+  </si>
+  <si>
+    <t>R30K ERJ-6ENF3002V</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF3002V</t>
+  </si>
+  <si>
+    <t>1=0.095, 10=0.0298, 50=0.0217, 100=0.0191, 500=0.0145, 1000=0.013, 5000=0.0102, 10000=0.0093, 250000=0.0088 (EUR)</t>
+  </si>
+  <si>
+    <t>ERJ6ENF3002V</t>
+  </si>
+  <si>
+    <t>1K 0805</t>
+  </si>
+  <si>
+    <t>Fixed Resistor, Metal Glaze/thick Film, 0.125W, 1000ohm, 150V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>R3, R7</t>
+  </si>
+  <si>
+    <t>R1K - RCA08051K00FKEA</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductors</t>
+  </si>
+  <si>
+    <t>RCA08051K00FKEA</t>
+  </si>
+  <si>
+    <t>10=0.0243, 50=0.0207, 100=0.0186, 500=0.0137, 1000=0.0118, 2500=0.0096, 5000=0.0082, 10000=0.007 (EUR)</t>
+  </si>
+  <si>
+    <t>19K1</t>
+  </si>
+  <si>
+    <t>Fixed Resistor, Metal Glaze/thick Film, 0.125W, 19100ohm, 150V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R19K1 ERJ-6ENF1912V</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1912V</t>
+  </si>
+  <si>
+    <t>1=0.1045, 10=0.0287, 50=0.0228, 100=0.0205, 5000=0.0089, 10000=0.0086 (EUR)</t>
+  </si>
+  <si>
+    <t>ERJ6ENF1912V</t>
+  </si>
+  <si>
+    <t>60K4 8085</t>
+  </si>
+  <si>
+    <t>Fixed Resistor, Metal Glaze/thick Film, 0.125W, 60400ohm, 150V, 1% +/-Tol, 100ppm/Cel, Surface Mount, 0805</t>
+  </si>
+  <si>
+    <t>R8, R9</t>
+  </si>
+  <si>
+    <t>R60K4 ERJ-6ENF6042V</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF6042V</t>
+  </si>
+  <si>
+    <t>1=0.0441, 50=0.0255, 100=0.0224, 250=0.0185, 500=0.0159, 1000=0.0136, 3000=0.0104, 5000=0.009, 10000=0.0086 (EUR)</t>
+  </si>
+  <si>
+    <t>ERJ6ENF6042V</t>
+  </si>
+  <si>
+    <t>SS22F03-G6</t>
+  </si>
+  <si>
+    <t>Slide switch DPDT 0.5A/50V</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SWDPDT-S22F03-G6</t>
+  </si>
+  <si>
+    <t>SW-SS22F03-G6</t>
+  </si>
+  <si>
+    <t>Ninigi</t>
+  </si>
+  <si>
+    <t>2=0.358, 5=0.303, 20=0.285, 100=0.257, 500=0.229 (EUR)</t>
   </si>
 </sst>
 </file>
@@ -166,15 +474,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,12 +496,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -196,6 +525,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,19 +866,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3290AB48-6F80-4228-9084-E2CC95644A7F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="85.5703125" customWidth="1"/>
+    <col min="1" max="2" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="85.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -557,7 +892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -585,7 +920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -599,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -613,7 +948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -627,7 +962,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -641,7 +976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -649,6 +984,511 @@
       <c r="C8" cm="1">
         <f t="array" ref="C8">SUM(B2:B7*C2:C7)</f>
         <v>174.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="6">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="6">
+        <v>2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="6">
+        <v>2</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -671,12 +1511,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +1524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -692,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -700,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -708,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -716,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -724,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -732,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -740,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -748,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>

</xml_diff>